<commit_message>
add soft/hard drop, animated fill, some optimizations
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nath/projects/tetris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FB84283F-C0EA-B740-810A-7AFC5F02C34B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F58BB59-3058-FC42-B5C7-F7679E9B3CE2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16160" activeTab="1" xr2:uid="{9124E530-86D9-CB42-81C4-694B9301110A}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16160" xr2:uid="{9124E530-86D9-CB42-81C4-694B9301110A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -659,6 +660,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Рисунок 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{993E8974-6014-1543-9876-418141F6A0AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1041400" y="0"/>
+          <a:ext cx="3403600" cy="7061200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Рисунок 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAB79930-46D1-3649-BCBC-7087A599923C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="203200"/>
+          <a:ext cx="3733800" cy="7137400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -958,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C40C3C1-E2E0-B542-971E-1EC27361E814}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
@@ -1320,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FC5B9B-3FDB-5148-B742-878116AD18EE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1330,4 +1424,19 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B500FC5-9761-EC42-824C-42871462A19B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>